<commit_message>
Testing Excel part 2.
</commit_message>
<xml_diff>
--- a/Contest.xlsx
+++ b/Contest.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="122211"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -25346,7 +25346,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Tag">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Tag">
   <location ref="I1:J43" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -25904,7 +25904,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G27" sqref="G27:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26433,6 +26433,9 @@
       <c r="D27" t="s">
         <v>28</v>
       </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
       <c r="I27" s="2" t="s">
         <v>49</v>
       </c>
@@ -26447,6 +26450,9 @@
       <c r="B28" t="s">
         <v>41</v>
       </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
       <c r="I28" s="2" t="s">
         <v>38</v>
       </c>
@@ -26460,6 +26466,9 @@
       </c>
       <c r="B29" t="s">
         <v>11</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>33</v>
@@ -26478,6 +26487,9 @@
       <c r="C30" t="s">
         <v>42</v>
       </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
       <c r="I30" s="2" t="s">
         <v>30</v>
       </c>
@@ -26495,6 +26507,9 @@
       <c r="C31" t="s">
         <v>44</v>
       </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
       <c r="I31" s="2" t="s">
         <v>21</v>
       </c>
@@ -26511,6 +26526,9 @@
       </c>
       <c r="C32" t="s">
         <v>46</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>42</v>

</xml_diff>